<commit_message>
Implemented method interceptor to run tests from excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/Test data.xlsx
+++ b/src/main/resources/Test data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/praveensharma/IdeaProjects/SeleniumAutomationFramework/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8D42F7-50F4-8F45-A215-D755819739D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3375D3-07B5-F049-9113-CFF3101DBD7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="14700" xr2:uid="{4FC76D2B-00FF-4148-9A4C-59EDF7983361}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="14700" activeTab="1" xr2:uid="{4FC76D2B-00FF-4148-9A4C-59EDF7983361}"/>
   </bookViews>
   <sheets>
     <sheet name="TestDataSheet" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Password</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>validateLoginPageTitle</t>
+  </si>
+  <si>
+    <t>validateLoginWithIncorrectCredentials</t>
   </si>
 </sst>
 </file>
@@ -112,7 +118,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEFAA6C-644B-A444-87D7-4BAE7B1B018B}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -468,10 +476,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7792FFFC-CBC5-4E45-8809-0FA894B39A5E}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -512,6 +520,22 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:2" ht="17">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="29">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>